<commit_message>
expanded db schema and about ot push to db
</commit_message>
<xml_diff>
--- a/docs/Video/Zeitplan.xlsx
+++ b/docs/Video/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\2425\ITP-Wettbewerbe-Website\docs\Video\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD73551-F2B9-411A-A5AE-2F2134542B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A0BB7B-4FC7-4399-A496-097EA7821BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA2BDFEA-A746-4547-AD12-9D3A65F03256}"/>
   </bookViews>
@@ -205,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -220,6 +220,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -554,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7F6BF8-A29D-43E6-B96A-26823D3ADA9D}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,115 +589,110 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>7</v>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5">
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E6" s="7">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>0.49305555555555558</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
         <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -706,11 +703,9 @@
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>8</v>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -721,48 +716,54 @@
       <c r="C11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
+      <c r="D11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9">
+      <c r="C13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3">
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
         <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7">
-        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,33 +776,33 @@
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9">
+      <c r="C17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9">
         <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,95 +815,119 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3">
         <v>20</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>45674</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="5">
-        <v>2</v>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="9">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="A25" s="11">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E25" s="9">
         <v>14</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>